<commit_message>
updated VM Plan template and VM Plan
</commit_message>
<xml_diff>
--- a/docs/vm_planning_template.xlsx
+++ b/docs/vm_planning_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vespe\source\repos\SQLServer_VENV\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{95CF69D5-899F-4DB9-87E3-D26C0EA2FBF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77E5186-81E5-41B0-A793-DAC9C97263B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29310" yWindow="1695" windowWidth="13695" windowHeight="14265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hypervisor Host" sheetId="1" r:id="rId1"/>
@@ -21,23 +21,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="71">
   <si>
     <t>Parameter</t>
   </si>
   <si>
-    <t>Value</t>
-  </si>
-  <si>
     <t>Host Name</t>
   </si>
   <si>
-    <t>Manufacturer</t>
-  </si>
-  <si>
-    <t>Model</t>
-  </si>
-  <si>
     <t>CPU Model</t>
   </si>
   <si>
@@ -53,18 +44,12 @@
     <t>RAM (GB)</t>
   </si>
   <si>
-    <t>ECC Memory (Yes/No)</t>
-  </si>
-  <si>
     <t>OS Version</t>
   </si>
   <si>
     <t>OS Edition</t>
   </si>
   <si>
-    <t>OS License Key</t>
-  </si>
-  <si>
     <t>Primary Disk Type (SSD/HDD/NVMe)</t>
   </si>
   <si>
@@ -80,12 +65,6 @@
     <t>Power Plan (High Performance/Other)</t>
   </si>
   <si>
-    <t>Secure Boot Enabled</t>
-  </si>
-  <si>
-    <t>Hyper-V Role Installed</t>
-  </si>
-  <si>
     <t>Update Status</t>
   </si>
   <si>
@@ -135,13 +114,158 @@
   </si>
   <si>
     <t>Provisioning Date</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>PowerShell (Admin) Command</t>
+  </si>
+  <si>
+    <t>Additional Logic</t>
+  </si>
+  <si>
+    <t>System Info</t>
+  </si>
+  <si>
+    <t>$env:COMPUTERNAME</t>
+  </si>
+  <si>
+    <t>System Manufacturer</t>
+  </si>
+  <si>
+    <t>Get-CimInstance Win32_ComputerSystem</t>
+  </si>
+  <si>
+    <t>System Model</t>
+  </si>
+  <si>
+    <t>Processor (CPU)</t>
+  </si>
+  <si>
+    <t>Get-CimInstance Win32_Processor</t>
+  </si>
+  <si>
+    <t>= physical cores x2</t>
+  </si>
+  <si>
+    <t>BIOS/UEFI Settings</t>
+  </si>
+  <si>
+    <t>systeminfo</t>
+  </si>
+  <si>
+    <t>Memory (RAM)</t>
+  </si>
+  <si>
+    <t>systeminfo -OR- Get-CimInstance Win32_ComputerSystem</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Windows reports storage in binary units (base 1024). Accounting for system reserved memory and memory rounding between binary (GiB) and decimal (GB) units, calculating gigs can be done by:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= bytes ÷ (1024³) = ~GB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. 
+Then round to the nearest whole number.</t>
+    </r>
+  </si>
+  <si>
+    <t>ECC Memory (True/False)</t>
+  </si>
+  <si>
+    <t>Get-CimInstance Win32_PhysicalMemory</t>
+  </si>
+  <si>
+    <t>If DataWidth = TotalWidth, then ECC is NOT enabled.</t>
+  </si>
+  <si>
+    <t>Get-CimInstance Win32_OperatingSystem</t>
+  </si>
+  <si>
+    <t>=CONCAT([Version] + "Build" + [BuildNumber])</t>
+  </si>
+  <si>
+    <t>Get-ItemProperty 'HKLM:\SOFTWARE\Microsoft\Windows NT\CurrentVersion</t>
+  </si>
+  <si>
+    <t>OS License Key / Activation Status</t>
+  </si>
+  <si>
+    <t>slmgr /xpr</t>
+  </si>
+  <si>
+    <t>If you use the license key, DON'T SHARE it. Only store in a secure, encrypted location. Otherwise consider putting "Yes/No" or Activation Status "Activated / Evaluation / Expired" in this field.</t>
+  </si>
+  <si>
+    <t>Storage</t>
+  </si>
+  <si>
+    <t>Get-PhysicalDisk</t>
+  </si>
+  <si>
+    <t>Network Interface Cards (NICs)</t>
+  </si>
+  <si>
+    <t>Get-NetAdapter | Where-Object { $_.Status -eq 'Up' -and $_.InterfaceDescription -notmatch 'Bluetooth' } | Measure-Object</t>
+  </si>
+  <si>
+    <t>Get-NetAdapter</t>
+  </si>
+  <si>
+    <t>powercfg /GETACTIVESCHEME</t>
+  </si>
+  <si>
+    <t>Secure Boot Enabled (True/False)</t>
+  </si>
+  <si>
+    <t>Confirm-SecureBootUEFI</t>
+  </si>
+  <si>
+    <t>Hyper-V Role Installed (True/False)</t>
+  </si>
+  <si>
+    <t>Get-WindowsOptionalFeature -FeatureName Microsoft-Hyper-V-All -Online</t>
+  </si>
+  <si>
+    <t>Available Updates</t>
+  </si>
+  <si>
+    <t>Get-WindowsUpdateLog</t>
+  </si>
+  <si>
+    <t>If no obvious signs of update failure, pending reboots, or errors in system logs, then it's up to date.</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>If nothing happens, the answer is False.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +281,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -166,7 +306,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -189,20 +329,147 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -213,6 +480,46 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C0782DE-1B62-414B-8BB1-20BCB0BD6131}" name="Table1" displayName="Table1" ref="A1:E22" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:E22" xr:uid="{2C0782DE-1B62-414B-8BB1-20BCB0BD6131}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{92126E60-4F28-4996-ACA6-DFF1810EDC3E}" name="Parameter" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{C25F6C41-C264-4416-A8DB-6CDF32F4C7BC}" name="Category"/>
+    <tableColumn id="3" xr3:uid="{235AF601-AECC-4219-9EBF-CC190026A562}" name="PowerShell (Admin) Command" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{CC5A141D-6976-4ABF-9F3B-FE6B4AF086AE}" name="Additional Logic" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{7ED22099-A1F2-4328-9D37-1245AA3E3FA9}" name="Values"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D65F76DA-B669-42B3-8C6B-E5DEA8B3D884}" name="Table3" displayName="Table3" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A1:Q2" xr:uid="{D65F76DA-B669-42B3-8C6B-E5DEA8B3D884}"/>
+  <tableColumns count="17">
+    <tableColumn id="1" xr3:uid="{02B1C0D7-B167-4A1D-87BD-E7A112BC1D1D}" name="VM Name"/>
+    <tableColumn id="2" xr3:uid="{13FAA0F3-5ECB-4E27-AC38-A96EA3BF3A03}" name="Environment (Dev/Test/Prod)"/>
+    <tableColumn id="3" xr3:uid="{CA425DCB-0C44-415E-BED2-A0C17612CD51}" name="Purpose / Role"/>
+    <tableColumn id="4" xr3:uid="{7C17CBD5-887A-4C47-80C6-CAC6A5A290E4}" name="vCPU Count"/>
+    <tableColumn id="5" xr3:uid="{ED2B4A29-11BD-4A4B-8E02-B34AB176BBCE}" name="RAM (GB)"/>
+    <tableColumn id="6" xr3:uid="{B21CD9CC-CF04-45F9-8B8A-EE0DEB8BC02A}" name="Storage - OS (GB)"/>
+    <tableColumn id="7" xr3:uid="{393C3598-7D7A-4327-961D-EF27573B95FA}" name="Storage - Data (GB)"/>
+    <tableColumn id="8" xr3:uid="{5D9524A1-034E-4664-8835-A2072C1CBCEE}" name="Expected IOPS"/>
+    <tableColumn id="9" xr3:uid="{387A7B61-9AF2-4581-86C1-12A4024B90A8}" name="Backup Policy"/>
+    <tableColumn id="10" xr3:uid="{180A31CD-46BA-4C72-ACE9-50E4F452A3B3}" name="Snapshot Schedule"/>
+    <tableColumn id="11" xr3:uid="{B1BA6D56-89CD-4DDE-9AFB-ABEF982C9618}" name="Operating System"/>
+    <tableColumn id="12" xr3:uid="{7EA5BD47-2755-403E-AF97-126D855CC755}" name="Software Installed"/>
+    <tableColumn id="13" xr3:uid="{7B144770-DE32-49C7-BC86-F2A1BB6A9392}" name="Network VLAN / IP"/>
+    <tableColumn id="14" xr3:uid="{3F34814C-73FB-456D-A356-67BC0F838988}" name="Priority (High/Med/Low)"/>
+    <tableColumn id="15" xr3:uid="{13D2B456-50B6-4F0F-93BB-2286754074FA}" name="Owner / Point of Contact"/>
+    <tableColumn id="16" xr3:uid="{D939B975-E113-430F-A2A0-05105CC35BCE}" name="Provisioning Date"/>
+    <tableColumn id="17" xr3:uid="{90C76EB3-B2FE-43DF-98E2-66F5D70DBB78}" name="Notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -502,131 +809,307 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.77734375" customWidth="1"/>
+    <col min="3" max="3" width="33.88671875" customWidth="1"/>
+    <col min="4" max="4" width="27.5546875" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" ht="144" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="B16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="B17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="B21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -634,64 +1117,87 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="J1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="K1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="L1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="M1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="N1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="O1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="P1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>22</v>
+      <c r="Q1" s="7" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>